<commit_message>
Update 05/10/2022 - Security
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Usuario</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Endpoint</t>
   </si>
   <si>
-    <t>PHE/Security-controller-adapter/1/Request 1</t>
-  </si>
-  <si>
     <t>Security Controller Adapter</t>
   </si>
   <si>
@@ -174,13 +171,40 @@
   </si>
   <si>
     <t>PHE/Security-certs-controller-adapter/Method 1/Request 1</t>
+  </si>
+  <si>
+    <t>Security/LoginToken</t>
+  </si>
+  <si>
+    <t>30-61398988-5</t>
+  </si>
+  <si>
+    <t>30-53725008-5</t>
+  </si>
+  <si>
+    <t>20-10474244-1</t>
+  </si>
+  <si>
+    <t>20-07608479-4</t>
+  </si>
+  <si>
+    <t>CUIT 1</t>
+  </si>
+  <si>
+    <t>CUIT 2</t>
+  </si>
+  <si>
+    <t>CUIT 3</t>
+  </si>
+  <si>
+    <t>CUIT 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,25 +218,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,12 +239,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -519,27 +528,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -547,7 +568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -555,7 +576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -563,7 +584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -571,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -579,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -587,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -595,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -603,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -611,7 +632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -619,15 +640,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -635,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -643,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -651,15 +672,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -667,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -675,12 +696,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +761,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,18 +780,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
         <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -778,15 +811,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -794,7 +827,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>401</v>
@@ -802,7 +835,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>403</v>
@@ -828,30 +861,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -878,23 +911,23 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 11/10/2022 BFF-Users GET Method
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
-    <sheet name="Servers" sheetId="2" r:id="rId2"/>
-    <sheet name="EndPoints" sheetId="3" r:id="rId3"/>
-    <sheet name="HTTPCodes" sheetId="4" r:id="rId4"/>
-    <sheet name="dBConnection" sheetId="5" r:id="rId5"/>
-    <sheet name="SQLStrings" sheetId="6" r:id="rId6"/>
+    <sheet name="Roles" sheetId="7" r:id="rId2"/>
+    <sheet name="Servers" sheetId="2" r:id="rId3"/>
+    <sheet name="EndPoints" sheetId="3" r:id="rId4"/>
+    <sheet name="HTTPCodes" sheetId="4" r:id="rId5"/>
+    <sheet name="dBConnection" sheetId="5" r:id="rId6"/>
+    <sheet name="SQLStrings" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>Usuario</t>
   </si>
@@ -170,9 +171,6 @@
     <t>Security Certs</t>
   </si>
   <si>
-    <t>PHE/Security-certs-controller-adapter/Method 1/Request 1</t>
-  </si>
-  <si>
     <t>Security/LoginToken</t>
   </si>
   <si>
@@ -198,6 +196,63 @@
   </si>
   <si>
     <t>CUIT 4</t>
+  </si>
+  <si>
+    <t>Users/Users</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>CID CUIT 1</t>
+  </si>
+  <si>
+    <t>CID CUIT 2</t>
+  </si>
+  <si>
+    <t>CID CUIT 3</t>
+  </si>
+  <si>
+    <t>CID CUIT 4</t>
+  </si>
+  <si>
+    <t>Conflict</t>
+  </si>
+  <si>
+    <t>Users/BFF-User</t>
+  </si>
+  <si>
+    <t>BFF User</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>ROLE_offline_access</t>
+  </si>
+  <si>
+    <t>ROLE_uma_authorization</t>
+  </si>
+  <si>
+    <t>ROLE_admin</t>
+  </si>
+  <si>
+    <t>ROLE_phe-free</t>
+  </si>
+  <si>
+    <t>Acceso offline</t>
+  </si>
+  <si>
+    <t>UMA Authorization</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>PayWay Free</t>
   </si>
 </sst>
 </file>
@@ -528,19 +583,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,19 +605,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -568,7 +640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -584,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -592,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -600,7 +672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -608,7 +680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -616,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -624,7 +696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -632,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -640,7 +712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -648,7 +720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -656,7 +728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -664,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -672,7 +744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -680,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -688,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -696,24 +768,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>51</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" t="s">
-        <v>53</v>
+      <c r="G19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19">
+        <v>1934</v>
+      </c>
+      <c r="I19">
+        <v>1933</v>
+      </c>
+      <c r="J19">
+        <v>1288</v>
+      </c>
+      <c r="K19">
+        <v>1809</v>
       </c>
     </row>
   </sheetData>
@@ -724,10 +811,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,12 +901,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +928,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,7 +936,15 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -799,12 +952,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,12 +994,20 @@
         <v>403</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>409</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -892,7 +1053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update 20/10/22:Agregado de eCommerce y Feature
</commit_message>
<xml_diff>
--- a/Test Data/MainData.xlsx
+++ b/Test Data/MainData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>Usuario</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Security Certs</t>
   </si>
   <si>
-    <t>Security/LoginToken</t>
-  </si>
-  <si>
     <t>30-61398988-5</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>CUIT 4</t>
   </si>
   <si>
-    <t>Users/Users</t>
-  </si>
-  <si>
     <t>Rol</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Conflict</t>
   </si>
   <si>
-    <t>Users/BFF-User</t>
-  </si>
-  <si>
     <t>BFF User</t>
   </si>
   <si>
@@ -253,6 +244,27 @@
   </si>
   <si>
     <t>PayWay Free</t>
+  </si>
+  <si>
+    <t>BFF User/Commerce</t>
+  </si>
+  <si>
+    <t>BFF Notification</t>
+  </si>
+  <si>
+    <t>03-Notification/Informaion Messages</t>
+  </si>
+  <si>
+    <t>01-Security/LoginToken</t>
+  </si>
+  <si>
+    <t>02-Users/Users</t>
+  </si>
+  <si>
+    <t>02-Users/BFF-User</t>
+  </si>
+  <si>
+    <t>02-Users/Commerce</t>
   </si>
 </sst>
 </file>
@@ -586,7 +598,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,31 +617,31 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>61</v>
-      </c>
-      <c r="J1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -776,19 +788,19 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
         <v>49</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>50</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>51</v>
       </c>
-      <c r="F19" t="s">
-        <v>52</v>
-      </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H19">
         <v>1934</v>
@@ -813,7 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -827,39 +839,39 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -903,10 +915,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +940,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,15 +948,31 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +1024,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>409</v>

</xml_diff>